<commit_message>
complete difference export support
</commit_message>
<xml_diff>
--- a/exports/B框-ppt-resource-container-web.xlsx
+++ b/exports/B框-ppt-resource-container-web.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -433,670 +433,568 @@
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>className.hot</v>
+        <v>disney.authorize_video</v>
       </c>
       <c r="B4" t="str">
-        <v>frameB-com-list__img-hot-cn</v>
+        <v>英语视频</v>
       </c>
       <c r="C4" t="str">
-        <v>frameB-com-list__img-hot</v>
+        <v>English video</v>
       </c>
       <c r="D4" t="str">
-        <v>frameB-com-list__img-hot</v>
+        <v>英語視頻</v>
       </c>
       <c r="E4" t="str">
-        <v>frameB-com-list__img-hot</v>
+        <v>فيديو عربي</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>className.boutique</v>
+        <v>disney.skin_center</v>
       </c>
       <c r="B5" t="str">
-        <v>frameB-com-list__img-boutique-cn</v>
+        <v>皮肤中心</v>
       </c>
       <c r="C5" t="str">
-        <v>frameB-com-list__img-boutique</v>
+        <v>Skin Center</v>
       </c>
       <c r="D5" t="str">
-        <v>frameB-com-list__img-boutique</v>
+        <v>皮膚中心</v>
       </c>
       <c r="E5" t="str">
-        <v>frameB-com-list__img-boutique</v>
+        <v>مركز الجلد</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>className.feature</v>
+        <v>disney.more_theme</v>
       </c>
       <c r="B6" t="str">
-        <v>frameB-com-list__img-feature-cn</v>
+        <v>更多主题</v>
       </c>
       <c r="C6" t="str">
-        <v>frameB-com-list__img-feature</v>
+        <v>More</v>
       </c>
       <c r="D6" t="str">
-        <v>frameB-com-list__img-feature</v>
+        <v>更多主題</v>
       </c>
       <c r="E6" t="str">
-        <v>frameB-com-list__img-feature</v>
+        <v>المزيد من المواضيع</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>className.news</v>
+        <v>disney.ipzone_placeholder</v>
       </c>
       <c r="B7" t="str">
-        <v>frameB-com-list__img-new-cn</v>
+        <v>搜索你想要的资源</v>
       </c>
       <c r="C7" t="str">
-        <v>frameB-com-list__img-new</v>
+        <v>Search for resources you want</v>
       </c>
       <c r="D7" t="str">
-        <v>frameB-com-list__img-new</v>
+        <v>搜索你想要的資源</v>
       </c>
       <c r="E7" t="str">
-        <v>frameB-com-list__img-new</v>
+        <v>البحث عن الموارد التي تريد</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>className.hard</v>
+        <v>disney.tips</v>
       </c>
       <c r="B8" t="str">
-        <v>icon-hard-cn</v>
+        <v>温馨提示</v>
       </c>
       <c r="C8" t="str">
-        <v>icon-hard</v>
+        <v>tips</v>
       </c>
       <c r="D8" t="str">
-        <v>icon-hard</v>
+        <v>溫馨提示</v>
       </c>
       <c r="E8" t="str">
-        <v>icon-hard</v>
+        <v>نصائح</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>audioItem.hot</v>
+        <v>disney.tips_desc</v>
       </c>
       <c r="B9" t="str">
-        <v>audio-container__hot-cn</v>
+        <v>您的版本过旧，无法插入最新资源，快去更新后体验吧~</v>
       </c>
       <c r="C9" t="str">
-        <v>audio-container__hot</v>
+        <v>Your version is too old to insert the latest resources. Go to update and experience it~</v>
       </c>
       <c r="D9" t="str">
-        <v>audio-container__hot</v>
+        <v>您的版本過舊，無法插入最新資源，快去更新後體驗吧~</v>
       </c>
       <c r="E9" t="str">
-        <v>audio-container__hot</v>
+        <v>أنت تستخدم إصدارًا منخفضًا جدًا. يُرجى ترقية الإصدار قبل استخدامه!</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>audioItem.boutique</v>
+        <v>disney.update_now</v>
       </c>
       <c r="B10" t="str">
-        <v>audio-container__boutique-cn</v>
+        <v>立即更新</v>
       </c>
       <c r="C10" t="str">
-        <v>audio-container__boutique</v>
+        <v>Update now</v>
       </c>
       <c r="D10" t="str">
-        <v>audio-container__boutique</v>
+        <v>立即更新</v>
       </c>
       <c r="E10" t="str">
-        <v>audio-container__boutique</v>
+        <v>تحديث فوري</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>audioItem.feature</v>
+        <v>disney.encourage_desc</v>
       </c>
       <c r="B11" t="str">
-        <v>audio-container__feature-cn</v>
+        <v>您可以在：放映态下 &gt; 互动工具 &gt; 表扬鼓励 &gt; 表扬工具 中进行体验</v>
       </c>
       <c r="C11" t="str">
-        <v>audio-container__feature</v>
+        <v>You can experience it in: Show &gt; Interactive Tools &gt; praise and encouragement &gt; praise tool</v>
       </c>
       <c r="D11" t="str">
-        <v>audio-container__feature</v>
+        <v>您可以在：放映態下 &gt; 互動工具 &gt; 表揚鼓勵 &gt; 表揚工具 中進行體驗</v>
       </c>
       <c r="E11" t="str">
-        <v>audio-container__feature</v>
+        <v>يمكنك تجربة مع أدوات تفاعلية في حالة العرض</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>audioItem.news</v>
+        <v>disney.team_competition</v>
       </c>
       <c r="B12" t="str">
-        <v>audio-container__new-cn</v>
+        <v>团队竞赛</v>
       </c>
       <c r="C12" t="str">
-        <v>audio-container__new</v>
+        <v>Team Competition</v>
       </c>
       <c r="D12" t="str">
-        <v>audio-container__new</v>
+        <v>團隊競賽</v>
       </c>
       <c r="E12" t="str">
-        <v>audio-container__new</v>
+        <v>فريق المنافسة</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>disney.authorize_video</v>
+        <v>disney.random_rollcall</v>
       </c>
       <c r="B13" t="str">
-        <v>英语视频</v>
+        <v>随机点名</v>
       </c>
       <c r="C13" t="str">
-        <v>English video</v>
+        <v>Random Roll Call</v>
       </c>
       <c r="D13" t="str">
-        <v>英語視頻</v>
+        <v>隨機點名</v>
       </c>
       <c r="E13" t="str">
-        <v>فيديو عربي</v>
+        <v>اسم عشوائي</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>disney.skin_center</v>
+        <v>disney.class_encourage</v>
       </c>
       <c r="B14" t="str">
-        <v>皮肤中心</v>
+        <v>课堂鼓励</v>
       </c>
       <c r="C14" t="str">
-        <v>Skin Center</v>
+        <v>Classroom Encouragement</v>
       </c>
       <c r="D14" t="str">
-        <v>皮膚中心</v>
+        <v>課堂鼓勵</v>
       </c>
       <c r="E14" t="str">
-        <v>مركز الجلد</v>
+        <v>تشجيع الفصول الدراسية</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>disney.more_theme</v>
+        <v>disney.disneyResponder</v>
       </c>
       <c r="B15" t="str">
-        <v>更多主题</v>
+        <v>抢答工具</v>
       </c>
       <c r="C15" t="str">
-        <v>More</v>
+        <v>Answer Tool</v>
       </c>
       <c r="D15" t="str">
-        <v>更多主題</v>
+        <v>搶答工具</v>
       </c>
       <c r="E15" t="str">
-        <v>المزيد من المواضيع</v>
+        <v>أداة الرد</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>disney.ipzone_placeholder</v>
+        <v>disney.encourage</v>
       </c>
       <c r="B16" t="str">
-        <v>搜索你想要的资源</v>
+        <v>鼓励</v>
       </c>
       <c r="C16" t="str">
-        <v>Search for resources you want</v>
+        <v>Encouragement</v>
       </c>
       <c r="D16" t="str">
-        <v>搜索你想要的資源</v>
+        <v>鼓勵</v>
       </c>
       <c r="E16" t="str">
-        <v>البحث عن الموارد التي تريد</v>
+        <v>شجع</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>disney.update_now</v>
+        <v>disney.responder</v>
       </c>
       <c r="B17" t="str">
-        <v>立即更新</v>
+        <v>抢答</v>
       </c>
       <c r="C17" t="str">
-        <v>Update now</v>
+        <v>Answer</v>
       </c>
       <c r="D17" t="str">
-        <v>立即更新</v>
+        <v>搶答</v>
       </c>
       <c r="E17" t="str">
-        <v>تحديث فوري</v>
+        <v>الرد السريع</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>disney.encourage_desc</v>
+        <v>disney.fl_remark</v>
       </c>
       <c r="B18" t="str">
-        <v>您可以在：放映态下 &gt; 互动工具 &gt; 表扬鼓励 &gt; 表扬工具 中进行体验</v>
+        <v>复仇者联盟邀你组队竞赛啦~</v>
       </c>
       <c r="C18" t="str">
-        <v>You can experience it in: Show &gt; Interactive Tools &gt; praise and encouragement &gt; praise tool</v>
+        <v>Avengers invite you to team up~</v>
       </c>
       <c r="D18" t="str">
-        <v>您可以在：放映態下 &gt; 互動工具 &gt; 表揚鼓勵 &gt; 表揚工具 中進行體驗</v>
+        <v>復仇者聯盟邀妳組隊競賽啦~</v>
       </c>
       <c r="E18" t="str">
-        <v>يمكنك تجربة مع أدوات تفاعلية في حالة العرض</v>
+        <v>دوري المنتقمون يدعوك إلى تنظيم المسابقة</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>disney.team_competition</v>
+        <v>disney.ml_remark</v>
       </c>
       <c r="B19" t="str">
-        <v>团队竞赛</v>
+        <v>可汗大点兵~抽学生课堂互动！</v>
       </c>
       <c r="C19" t="str">
-        <v>Team Competition</v>
+        <v>Khan big spot soldier ~ smoke student classroom interaction!</v>
       </c>
       <c r="D19" t="str">
-        <v>團隊競賽</v>
+        <v>可汗大點兵~抽學生課堂互動！</v>
       </c>
       <c r="E19" t="str">
-        <v>فريق المنافسة</v>
+        <v>ما هو نوع من التفاعل الصفي ؟</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>disney.random_rollcall</v>
+        <v>disney.bx_remark</v>
       </c>
       <c r="B20" t="str">
-        <v>随机点名</v>
+        <v>放映态下&gt;互动工具&gt;表扬</v>
       </c>
       <c r="C20" t="str">
-        <v>Random Roll Call</v>
+        <v>Show &gt; Interactive Tools &gt; praise</v>
       </c>
       <c r="D20" t="str">
-        <v>隨機點名</v>
+        <v>放映態下&gt;互動工具&gt;表揚</v>
       </c>
       <c r="E20" t="str">
-        <v>اسم عشوائي</v>
+        <v>أداة تفاعلية في حالة العرض</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>disney.class_encourage</v>
+        <v>disney.mq_remark</v>
       </c>
       <c r="B21" t="str">
-        <v>课堂鼓励</v>
+        <v>与赛车手米奇一起抢答吧~</v>
       </c>
       <c r="C21" t="str">
-        <v>Classroom Encouragement</v>
+        <v>Join race car driver Mickey in the contest~</v>
       </c>
       <c r="D21" t="str">
-        <v>課堂鼓勵</v>
+        <v>與賽車手米奇壹起搶答吧~</v>
       </c>
       <c r="E21" t="str">
-        <v>تشجيع الفصول الدراسية</v>
+        <v>مع ميكي ، متسابق</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>disney.disneyResponder</v>
+        <v>disney.use_now</v>
       </c>
       <c r="B22" t="str">
-        <v>抢答工具</v>
+        <v>立即使用</v>
       </c>
       <c r="C22" t="str">
-        <v>Answer Tool</v>
+        <v>Use it now</v>
       </c>
       <c r="D22" t="str">
-        <v>搶答工具</v>
+        <v>立即使用</v>
       </c>
       <c r="E22" t="str">
-        <v>أداة الرد</v>
+        <v>استخدام فوري</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>disney.encourage</v>
+        <v>disney.login_use</v>
       </c>
       <c r="B23" t="str">
-        <v>鼓励</v>
+        <v>登录后即可使用</v>
       </c>
       <c r="C23" t="str">
-        <v>Encouragement</v>
+        <v>Please log in</v>
       </c>
       <c r="D23" t="str">
-        <v>鼓勵</v>
+        <v>登錄後即可使用</v>
       </c>
       <c r="E23" t="str">
-        <v>شجع</v>
+        <v>بعد تسجيل الدخول يمكنك استخدام</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>disney.responder</v>
+        <v>disney.resource</v>
       </c>
       <c r="B24" t="str">
-        <v>抢答</v>
+        <v>资源类型</v>
       </c>
       <c r="C24" t="str">
-        <v>Answer</v>
+        <v>Resource Type</v>
       </c>
       <c r="D24" t="str">
-        <v>搶答</v>
+        <v>資源類型</v>
       </c>
       <c r="E24" t="str">
-        <v>الرد السريع</v>
+        <v>أنواع الموارد</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>disney.fl_remark</v>
+        <v>disney.current</v>
       </c>
       <c r="B25" t="str">
-        <v>复仇者联盟邀你组队竞赛啦~</v>
+        <v>当前</v>
       </c>
       <c r="C25" t="str">
-        <v>Avengers invite you to team up~</v>
+        <v>Current</v>
       </c>
       <c r="D25" t="str">
-        <v>復仇者聯盟邀妳組隊競賽啦~</v>
+        <v>當前</v>
       </c>
       <c r="E25" t="str">
-        <v>دوري المنتقمون يدعوك إلى تنظيم المسابقة</v>
+        <v>حالي</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>disney.ml_remark</v>
+        <v>disney.ipzone</v>
       </c>
       <c r="B26" t="str">
-        <v>可汗大点兵~抽学生课堂互动！</v>
+        <v>迪士尼专区</v>
       </c>
       <c r="C26" t="str">
-        <v>Khan big spot soldier ~ smoke student classroom interaction!</v>
+        <v>Disney Zone</v>
       </c>
       <c r="D26" t="str">
-        <v>可汗大點兵~抽學生課堂互動！</v>
+        <v>迪士尼專區</v>
       </c>
       <c r="E26" t="str">
-        <v>ما هو نوع من التفاعل الصفي ؟</v>
+        <v>ديزني لاند</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>disney.bx_remark</v>
+        <v>globalSearch.exercise</v>
       </c>
       <c r="B27" t="str">
-        <v>放映态下&gt;互动工具&gt;表扬</v>
+        <v>习题/试卷</v>
       </c>
       <c r="C27" t="str">
-        <v>Show &gt; Interactive Tools &gt; praise</v>
+        <v>Exercises &amp; Test Papers</v>
       </c>
       <c r="D27" t="str">
-        <v>放映態下&gt;互動工具&gt;表揚</v>
+        <v>習題/試卷</v>
       </c>
       <c r="E27" t="str">
-        <v>أداة تفاعلية في حالة العرض</v>
+        <v>رياضي</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>disney.mq_remark</v>
+        <v>authorWorks.activity_homepage</v>
       </c>
       <c r="B28" t="str">
-        <v>与赛车手米奇一起抢答吧~</v>
+        <v>活动首页</v>
       </c>
       <c r="C28" t="str">
-        <v>Join race car driver Mickey in the contest~</v>
+        <v>home</v>
       </c>
       <c r="D28" t="str">
-        <v>與賽車手米奇壹起搶答吧~</v>
+        <v>活動首頁</v>
       </c>
       <c r="E28" t="str">
-        <v>مع ميكي ، متسابق</v>
+        <v>الصفحة الرئيسية النشطة</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>disney.use_now</v>
+        <v>authorWorks.my_works</v>
       </c>
       <c r="B29" t="str">
-        <v>立即使用</v>
+        <v>我的参赛作品</v>
       </c>
       <c r="C29" t="str">
-        <v>Use it now</v>
+        <v>My entries</v>
       </c>
       <c r="D29" t="str">
-        <v>立即使用</v>
+        <v>我的參賽作品</v>
       </c>
       <c r="E29" t="str">
-        <v>استخدام فوري</v>
+        <v>بلدي يعمل</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>disney.login_use</v>
+        <v>authorWorks.my_selected_works</v>
       </c>
       <c r="B30" t="str">
-        <v>登录后即可使用</v>
+        <v>我的入选作品集</v>
       </c>
       <c r="C30" t="str">
-        <v>Please log in</v>
+        <v>Selected works</v>
       </c>
       <c r="D30" t="str">
-        <v>登錄後即可使用</v>
+        <v>我的入選作品集</v>
       </c>
       <c r="E30" t="str">
-        <v>بعد تسجيل الدخول يمكنك استخدام</v>
+        <v>بلدي مجموعة مختارة</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>disney.resource</v>
+        <v>authorWorks.selected_works</v>
       </c>
       <c r="B31" t="str">
-        <v>资源类型</v>
+        <v>入选作品</v>
       </c>
       <c r="C31" t="str">
-        <v>Resource Type</v>
+        <v>selected</v>
       </c>
       <c r="D31" t="str">
-        <v>資源類型</v>
+        <v>入選作品</v>
       </c>
       <c r="E31" t="str">
-        <v>أنواع الموارد</v>
+        <v>أعمال مختارة</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v>disney.current</v>
+        <v>authorWorks.award_works</v>
       </c>
       <c r="B32" t="str">
-        <v>当前</v>
+        <v>获奖作品</v>
       </c>
       <c r="C32" t="str">
-        <v>Current</v>
+        <v>prize</v>
       </c>
       <c r="D32" t="str">
-        <v>當前</v>
+        <v>獲獎作品</v>
       </c>
       <c r="E32" t="str">
-        <v>حالي</v>
+        <v>الحائز على جائزة العمل</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>disney.ipzone</v>
+        <v>authorWorks.praise</v>
       </c>
       <c r="B33" t="str">
-        <v>迪士尼专区</v>
+        <v>收获赞</v>
       </c>
       <c r="C33" t="str">
-        <v>Disney Zone</v>
+        <v>praise</v>
       </c>
       <c r="D33" t="str">
-        <v>迪士尼專區</v>
+        <v>收穫贊</v>
       </c>
       <c r="E33" t="str">
-        <v>ديزني لاند</v>
+        <v>حصاد الحمد</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>authorWorks.activity_homepage</v>
+        <v>authorWorks.used</v>
       </c>
       <c r="B34" t="str">
-        <v>活动首页</v>
+        <v>被使用</v>
       </c>
       <c r="C34" t="str">
-        <v>home</v>
+        <v>used</v>
       </c>
       <c r="D34" t="str">
-        <v>活動首頁</v>
+        <v>被使用</v>
       </c>
       <c r="E34" t="str">
-        <v>الصفحة الرئيسية النشطة</v>
+        <v>تستخدم</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>authorWorks.my_works</v>
+        <v>authorWorks.no_more</v>
       </c>
       <c r="B35" t="str">
-        <v>我的参赛作品</v>
+        <v>没有更多了</v>
       </c>
       <c r="C35" t="str">
-        <v>My entries</v>
+        <v>no more</v>
       </c>
       <c r="D35" t="str">
-        <v>我的參賽作品</v>
+        <v>沒有更多了</v>
       </c>
       <c r="E35" t="str">
-        <v>بلدي يعمل</v>
+        <v>لا أكثر</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v>authorWorks.my_selected_works</v>
+        <v>authorWorks.take_part_in</v>
       </c>
       <c r="B36" t="str">
-        <v>我的入选作品集</v>
+        <v>加入作品征集大赛，共建教学资源库</v>
       </c>
       <c r="C36" t="str">
-        <v>Selected works</v>
+        <v>Join the competition of collecting works and build a teaching resource library</v>
       </c>
       <c r="D36" t="str">
-        <v>我的入選作品集</v>
+        <v>加入作品徵集大賽，共建教學資源庫</v>
       </c>
       <c r="E36" t="str">
-        <v>بلدي مجموعة مختارة</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="str">
-        <v>authorWorks.selected_works</v>
-      </c>
-      <c r="B37" t="str">
-        <v>入选作品</v>
-      </c>
-      <c r="C37" t="str">
-        <v>selected</v>
-      </c>
-      <c r="D37" t="str">
-        <v>入選作品</v>
-      </c>
-      <c r="E37" t="str">
-        <v>أعمال مختارة</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="str">
-        <v>authorWorks.award_works</v>
-      </c>
-      <c r="B38" t="str">
-        <v>获奖作品</v>
-      </c>
-      <c r="C38" t="str">
-        <v>prize</v>
-      </c>
-      <c r="D38" t="str">
-        <v>獲獎作品</v>
-      </c>
-      <c r="E38" t="str">
-        <v>الحائز على جائزة العمل</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="str">
-        <v>authorWorks.praise</v>
-      </c>
-      <c r="B39" t="str">
-        <v>收获赞</v>
-      </c>
-      <c r="C39" t="str">
-        <v>praise</v>
-      </c>
-      <c r="D39" t="str">
-        <v>收穫贊</v>
-      </c>
-      <c r="E39" t="str">
-        <v>حصاد الحمد</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="str">
-        <v>authorWorks.used</v>
-      </c>
-      <c r="B40" t="str">
-        <v>被使用</v>
-      </c>
-      <c r="C40" t="str">
-        <v>used</v>
-      </c>
-      <c r="D40" t="str">
-        <v>被使用</v>
-      </c>
-      <c r="E40" t="str">
-        <v>تستخدم</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="str">
-        <v>authorWorks.no_more</v>
-      </c>
-      <c r="B41" t="str">
-        <v>没有更多了</v>
-      </c>
-      <c r="C41" t="str">
-        <v>no more</v>
-      </c>
-      <c r="D41" t="str">
-        <v>沒有更多了</v>
-      </c>
-      <c r="E41" t="str">
-        <v>لا أكثر</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="str">
-        <v>authorWorks.take_part_in</v>
-      </c>
-      <c r="B42" t="str">
-        <v>加入作品征集大赛，共建教学资源库</v>
-      </c>
-      <c r="C42" t="str">
-        <v>Join the competition of collecting works and build a teaching resource library</v>
-      </c>
-      <c r="D42" t="str">
-        <v>加入作品徵集大賽，共建教學資源庫</v>
-      </c>
-      <c r="E42" t="str">
         <v>الانضمام إلى مسابقة جمع الأعمال ، وبناء قاعدة بيانات الموارد التعليمية</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E42"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E36"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>